<commit_message>
[feat] update excel data
</commit_message>
<xml_diff>
--- a/Util/ExcelToJsonWizard.v1.0.6/excel_files/Enum.xlsx
+++ b/Util/ExcelToJsonWizard.v1.0.6/excel_files/Enum.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROJECTS\UNITY_PROJECTS\ProjectI\Util\ExcelToJsonWizard.v1.0.6\excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8721EF0-C99B-44CA-82DE-FAD58EC89979}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B272C1E-73D6-4EB8-9459-D72E46BB3361}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31875" yWindow="1785" windowWidth="19320" windowHeight="17055" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="38700" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Grade</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -110,10 +110,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Heart</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>BlackHeart</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -123,6 +119,26 @@
   </si>
   <si>
     <t>SoulHeart</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Coin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Boom</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Key</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CurHeart</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MaxHeart</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -451,10 +467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="A3:B3"/>
+      <selection activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -464,7 +480,7 @@
     <col min="4" max="4" width="11.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -487,7 +503,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="33" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" ht="33" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -516,22 +532,34 @@
         <v>9</v>
       </c>
       <c r="J2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>21</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>